<commit_message>
Third Commit - Bruins Forwards Data
</commit_message>
<xml_diff>
--- a/bruins/2023_bruins_goalies_regular_season.xlsx
+++ b/bruins/2023_bruins_goalies_regular_season.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AD4"/>
+  <dimension ref="A1:AC4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,145 +436,140 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Rk</t>
+          <t>Player</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Player</t>
+          <t>Age</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Age</t>
+          <t>Pos</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Pos</t>
+          <t>GP</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>GP</t>
+          <t>G</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>G</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>PTS</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>PTS</t>
+          <t>+/-</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>+/-</t>
+          <t>PIM</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>PIM</t>
+          <t>EV</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>EV</t>
+          <t>PP</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>PP</t>
+          <t>SH</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>SH</t>
+          <t>GW</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>GW</t>
+          <t>EV.1</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>EV.1</t>
+          <t>PP.1</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>PP.1</t>
+          <t>SH.1</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>SH.1</t>
+          <t>S</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>S%</t>
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
-          <t>S%</t>
+          <t>TOI</t>
         </is>
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
-          <t>TOI</t>
+          <t>ATOI</t>
         </is>
       </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
-          <t>ATOI</t>
+          <t>OPS</t>
         </is>
       </c>
       <c r="W1" s="1" t="inlineStr">
         <is>
-          <t>OPS</t>
+          <t>DPS</t>
         </is>
       </c>
       <c r="X1" s="1" t="inlineStr">
         <is>
-          <t>DPS</t>
+          <t>PS</t>
         </is>
       </c>
       <c r="Y1" s="1" t="inlineStr">
         <is>
-          <t>PS</t>
+          <t>BLK</t>
         </is>
       </c>
       <c r="Z1" s="1" t="inlineStr">
         <is>
-          <t>BLK</t>
+          <t>HIT</t>
         </is>
       </c>
       <c r="AA1" s="1" t="inlineStr">
         <is>
-          <t>HIT</t>
+          <t>FOW</t>
         </is>
       </c>
       <c r="AB1" s="1" t="inlineStr">
         <is>
-          <t>FOW</t>
+          <t>FOL</t>
         </is>
       </c>
       <c r="AC1" s="1" t="inlineStr">
-        <is>
-          <t>FOL</t>
-        </is>
-      </c>
-      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>FO%</t>
         </is>
@@ -584,83 +579,83 @@
       <c r="A2" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="B2" t="n">
-        <v>26</v>
-      </c>
-      <c r="C2" t="inlineStr">
+      <c r="B2" t="inlineStr">
         <is>
           <t>Linus Ullmark</t>
         </is>
       </c>
-      <c r="D2" t="n">
+      <c r="C2" t="n">
         <v>29</v>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>G</t>
         </is>
       </c>
+      <c r="E2" t="n">
+        <v>49</v>
+      </c>
       <c r="F2" t="n">
-        <v>49</v>
+        <v>1</v>
       </c>
       <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
         <v>1</v>
       </c>
-      <c r="H2" t="n">
-        <v>0</v>
-      </c>
       <c r="I2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>2</v>
+      </c>
+      <c r="K2" t="n">
         <v>1</v>
       </c>
-      <c r="J2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K2" t="n">
-        <v>2</v>
-      </c>
       <c r="L2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R2" t="n">
         <v>1</v>
       </c>
-      <c r="M2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>0</v>
-      </c>
-      <c r="R2" t="n">
-        <v>0</v>
-      </c>
       <c r="S2" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="T2" t="n">
-        <v>100</v>
-      </c>
-      <c r="U2" t="n">
         <v>2882</v>
       </c>
-      <c r="V2" t="inlineStr">
+      <c r="U2" t="inlineStr">
         <is>
           <t>58:49</t>
         </is>
       </c>
+      <c r="V2" t="n">
+        <v>0</v>
+      </c>
       <c r="W2" t="n">
         <v>0</v>
       </c>
       <c r="X2" t="n">
-        <v>0</v>
+        <v>13.2</v>
       </c>
       <c r="Y2" t="n">
-        <v>13.2</v>
+        <v>0</v>
       </c>
       <c r="Z2" t="n">
         <v>0</v>
@@ -671,33 +666,30 @@
       <c r="AB2" t="n">
         <v>0</v>
       </c>
-      <c r="AC2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD2" t="inlineStr"/>
+      <c r="AC2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="B3" t="n">
-        <v>30</v>
-      </c>
-      <c r="C3" t="inlineStr">
+      <c r="B3" t="inlineStr">
         <is>
           <t>Keith Kinkaid</t>
         </is>
       </c>
-      <c r="D3" t="n">
+      <c r="C3" t="n">
         <v>33</v>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>G</t>
         </is>
       </c>
+      <c r="E3" t="n">
+        <v>1</v>
+      </c>
       <c r="F3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
@@ -705,10 +697,10 @@
       <c r="H3" t="n">
         <v>0</v>
       </c>
-      <c r="I3" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="n">
+        <v>0</v>
+      </c>
       <c r="K3" t="n">
         <v>0</v>
       </c>
@@ -733,26 +725,26 @@
       <c r="R3" t="n">
         <v>0</v>
       </c>
-      <c r="S3" t="n">
-        <v>0</v>
-      </c>
-      <c r="T3" t="inlineStr"/>
-      <c r="U3" t="n">
+      <c r="S3" t="inlineStr"/>
+      <c r="T3" t="n">
         <v>60</v>
       </c>
-      <c r="V3" t="inlineStr">
+      <c r="U3" t="inlineStr">
         <is>
           <t>59:54</t>
         </is>
       </c>
+      <c r="V3" t="n">
+        <v>0</v>
+      </c>
       <c r="W3" t="n">
         <v>0</v>
       </c>
       <c r="X3" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="Z3" t="n">
         <v>0</v>
@@ -763,33 +755,30 @@
       <c r="AB3" t="n">
         <v>0</v>
       </c>
-      <c r="AC3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD3" t="inlineStr"/>
+      <c r="AC3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="B4" t="n">
-        <v>36</v>
-      </c>
-      <c r="C4" t="inlineStr">
+      <c r="B4" t="inlineStr">
         <is>
           <t>Jeremy Swayman</t>
         </is>
       </c>
-      <c r="D4" t="n">
+      <c r="C4" t="n">
         <v>24</v>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>G</t>
         </is>
       </c>
+      <c r="E4" t="n">
+        <v>37</v>
+      </c>
       <c r="F4" t="n">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="G4" t="n">
         <v>0</v>
@@ -801,10 +790,10 @@
         <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L4" t="n">
         <v>0</v>
@@ -827,26 +816,26 @@
       <c r="R4" t="n">
         <v>0</v>
       </c>
-      <c r="S4" t="n">
-        <v>0</v>
-      </c>
-      <c r="T4" t="inlineStr"/>
-      <c r="U4" t="n">
+      <c r="S4" t="inlineStr"/>
+      <c r="T4" t="n">
         <v>2013</v>
       </c>
-      <c r="V4" t="inlineStr">
+      <c r="U4" t="inlineStr">
         <is>
           <t>54:24</t>
         </is>
       </c>
+      <c r="V4" t="n">
+        <v>0</v>
+      </c>
       <c r="W4" t="n">
         <v>0</v>
       </c>
       <c r="X4" t="n">
-        <v>0</v>
+        <v>6.9</v>
       </c>
       <c r="Y4" t="n">
-        <v>6.9</v>
+        <v>0</v>
       </c>
       <c r="Z4" t="n">
         <v>0</v>
@@ -857,10 +846,7 @@
       <c r="AB4" t="n">
         <v>0</v>
       </c>
-      <c r="AC4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD4" t="inlineStr"/>
+      <c r="AC4" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>